<commit_message>
fixed issue where i had forgotten to add the MatOR material to the materials set when it was not found as a key in the sorted product dict
</commit_message>
<xml_diff>
--- a/Test Folder/z - BALL - Hinge Boring Script - TEST/z - BALL - Hinge Boring Script - TEST - Hinge Boring List.xlsx
+++ b/Test Folder/z - BALL - Hinge Boring Script - TEST/z - BALL - Hinge Boring Script - TEST - Hinge Boring List.xlsx
@@ -1273,7 +1273,7 @@
       </c>
       <c r="M28" s="9" t="inlineStr">
         <is>
-          <t>R1C10</t>
+          <t>R1C9</t>
         </is>
       </c>
     </row>
@@ -1719,7 +1719,7 @@
       </c>
       <c r="M38" s="7" t="inlineStr">
         <is>
-          <t>R1C9</t>
+          <t>R1C10</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed error where material was being set as MatOR on the first instance when it was not None and then never reset to the room material
</commit_message>
<xml_diff>
--- a/Test Folder/z - BALL - Hinge Boring Script - TEST/z - BALL - Hinge Boring Script - TEST - Hinge Boring List.xlsx
+++ b/Test Folder/z - BALL - Hinge Boring Script - TEST/z - BALL - Hinge Boring Script - TEST - Hinge Boring List.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Sheet'!$A$1:$M$127</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Sheet'!$A$1:$M$156</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -492,7 +492,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M127"/>
+  <dimension ref="A1:M156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -602,7 +602,7 @@
       </c>
       <c r="K7" s="6" t="inlineStr">
         <is>
-          <t>T2/R2</t>
+          <t>B3/L3</t>
         </is>
       </c>
       <c r="L7" s="6" t="inlineStr">
@@ -733,7 +733,7 @@
       </c>
       <c r="K12" s="6" t="inlineStr">
         <is>
-          <t>T2/R2</t>
+          <t>B3/L3</t>
         </is>
       </c>
       <c r="L12" s="6" t="inlineStr">
@@ -908,7 +908,7 @@
       </c>
       <c r="K18" s="6" t="inlineStr">
         <is>
-          <t>T2/R2</t>
+          <t>B3/L3</t>
         </is>
       </c>
       <c r="L18" s="6" t="inlineStr">
@@ -1039,7 +1039,7 @@
       </c>
       <c r="K23" s="6" t="inlineStr">
         <is>
-          <t>T2/R2</t>
+          <t>B3/L3</t>
         </is>
       </c>
       <c r="L23" s="6" t="inlineStr">
@@ -1266,7 +1266,7 @@
         <v>367.2</v>
       </c>
       <c r="K28" s="9" t="n">
-        <v>291</v>
+        <v>582.1</v>
       </c>
       <c r="L28" s="9" t="n">
         <v>101.6</v>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="K50" s="6" t="inlineStr">
         <is>
-          <t>T2/R2</t>
+          <t>B3/L3</t>
         </is>
       </c>
       <c r="L50" s="6" t="inlineStr">
@@ -2533,7 +2533,7 @@
       </c>
       <c r="K68" s="6" t="inlineStr">
         <is>
-          <t>T2/R2</t>
+          <t>B3/L3</t>
         </is>
       </c>
       <c r="L68" s="6" t="inlineStr">
@@ -2664,7 +2664,7 @@
       </c>
       <c r="K73" s="6" t="inlineStr">
         <is>
-          <t>T2/R2</t>
+          <t>B3/L3</t>
         </is>
       </c>
       <c r="L73" s="6" t="inlineStr">
@@ -2839,7 +2839,7 @@
       </c>
       <c r="K79" s="6" t="inlineStr">
         <is>
-          <t>T2/R2</t>
+          <t>B3/L3</t>
         </is>
       </c>
       <c r="L79" s="6" t="inlineStr">
@@ -2923,21 +2923,21 @@
     <row r="87" ht="18" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>02 - PAN - Absolute Acajou</t>
+          <t>02 - AGT - White Gloss</t>
         </is>
       </c>
     </row>
     <row r="89" ht="18" customHeight="1">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>Shaker Door</t>
+          <t>Slab Door - VG</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="B91" s="4" t="inlineStr">
         <is>
-          <t>DTC C-80 110 / 2mm - 105-C80A675NF</t>
+          <t>Blum 95 Blind / 3mm - 79B958180</t>
         </is>
       </c>
       <c r="C91" s="5" t="n"/>
@@ -3000,7 +3000,7 @@
       </c>
       <c r="K92" s="6" t="inlineStr">
         <is>
-          <t>T2/R2</t>
+          <t>B3/L3</t>
         </is>
       </c>
       <c r="L92" s="6" t="inlineStr">
@@ -3015,628 +3015,1408 @@
       </c>
     </row>
     <row r="93">
-      <c r="B93" s="8" t="inlineStr">
-        <is>
-          <t>Hinge Type Total: (0)</t>
+      <c r="B93" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C93" s="7" t="inlineStr">
+        <is>
+          <t>Door(R)</t>
+        </is>
+      </c>
+      <c r="D93" s="7" t="inlineStr">
+        <is>
+          <t>Cabinet Door</t>
+        </is>
+      </c>
+      <c r="E93" s="7" t="n">
+        <v>314.3</v>
+      </c>
+      <c r="F93" s="7" t="n">
+        <v>912.8</v>
+      </c>
+      <c r="G93" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="H93" s="7" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
+      <c r="I93" s="7" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="J93" s="7" t="inlineStr"/>
+      <c r="K93" s="7" t="inlineStr"/>
+      <c r="L93" s="7" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="M93" s="7" t="inlineStr">
+        <is>
+          <t>R3C10</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="B94" s="8" t="inlineStr">
+        <is>
+          <t>Hinge Type Total: (1)</t>
         </is>
       </c>
     </row>
     <row r="96">
-      <c r="B96" s="10" t="inlineStr">
-        <is>
-          <t>Door Style Total: (0)</t>
+      <c r="B96" s="4" t="inlineStr">
+        <is>
+          <t>DTC C-80 110 / 2mm - 105-C80A675NF</t>
         </is>
       </c>
       <c r="C96" s="5" t="n"/>
       <c r="D96" s="5" t="n"/>
-    </row>
-    <row r="98" ht="18" customHeight="1">
-      <c r="A98" s="3" t="inlineStr">
+      <c r="E96" s="5" t="n"/>
+      <c r="F96" s="5" t="n"/>
+      <c r="G96" s="5" t="n"/>
+      <c r="H96" s="5" t="n"/>
+      <c r="I96" s="5" t="n"/>
+      <c r="J96" s="5" t="n"/>
+      <c r="K96" s="5" t="n"/>
+      <c r="L96" s="5" t="n"/>
+      <c r="M96" s="5" t="n"/>
+    </row>
+    <row r="97">
+      <c r="B97" s="6" t="inlineStr">
+        <is>
+          <t>Qty</t>
+        </is>
+      </c>
+      <c r="C97" s="6" t="inlineStr">
+        <is>
+          <t>Door Name</t>
+        </is>
+      </c>
+      <c r="D97" s="6" t="inlineStr">
+        <is>
+          <t>Comment</t>
+        </is>
+      </c>
+      <c r="E97" s="6" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="F97" s="6" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="G97" s="6" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="H97" s="6" t="inlineStr">
+        <is>
+          <t>Edge</t>
+        </is>
+      </c>
+      <c r="I97" s="6" t="inlineStr">
+        <is>
+          <t>B/L</t>
+        </is>
+      </c>
+      <c r="J97" s="6" t="inlineStr">
+        <is>
+          <t>B2/L2</t>
+        </is>
+      </c>
+      <c r="K97" s="6" t="inlineStr">
+        <is>
+          <t>B3/L3</t>
+        </is>
+      </c>
+      <c r="L97" s="6" t="inlineStr">
+        <is>
+          <t>T/R</t>
+        </is>
+      </c>
+      <c r="M97" s="6" t="inlineStr">
+        <is>
+          <t>Cab #</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="B98" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C98" s="9" t="inlineStr">
+        <is>
+          <t>Door(L)</t>
+        </is>
+      </c>
+      <c r="D98" s="9" t="inlineStr">
+        <is>
+          <t>Cabinet Door</t>
+        </is>
+      </c>
+      <c r="E98" s="9" t="n">
+        <v>377.8</v>
+      </c>
+      <c r="F98" s="9" t="n">
+        <v>492.1</v>
+      </c>
+      <c r="G98" s="9" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H98" s="9" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="I98" s="9" t="n">
+        <v>63.5</v>
+      </c>
+      <c r="J98" s="9" t="inlineStr"/>
+      <c r="K98" s="9" t="inlineStr"/>
+      <c r="L98" s="9" t="n">
+        <v>63.5</v>
+      </c>
+      <c r="M98" s="9" t="inlineStr">
+        <is>
+          <t>R3C12</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="B99" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C99" s="9" t="inlineStr">
+        <is>
+          <t>Door(R)</t>
+        </is>
+      </c>
+      <c r="D99" s="9" t="inlineStr">
+        <is>
+          <t>Cabinet Door</t>
+        </is>
+      </c>
+      <c r="E99" s="9" t="n">
+        <v>377.8</v>
+      </c>
+      <c r="F99" s="9" t="n">
+        <v>492.1</v>
+      </c>
+      <c r="G99" s="9" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H99" s="9" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
+      <c r="I99" s="9" t="n">
+        <v>63.5</v>
+      </c>
+      <c r="J99" s="9" t="inlineStr"/>
+      <c r="K99" s="9" t="inlineStr"/>
+      <c r="L99" s="9" t="n">
+        <v>63.5</v>
+      </c>
+      <c r="M99" s="9" t="inlineStr">
+        <is>
+          <t>R3C12</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="B100" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C100" s="9" t="inlineStr">
+        <is>
+          <t>Door(L)</t>
+        </is>
+      </c>
+      <c r="D100" s="9" t="inlineStr">
+        <is>
+          <t>Cabinet Door</t>
+        </is>
+      </c>
+      <c r="E100" s="9" t="n">
+        <v>435</v>
+      </c>
+      <c r="F100" s="9" t="n">
+        <v>606.4</v>
+      </c>
+      <c r="G100" s="9" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="H100" s="9" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="I100" s="9" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="J100" s="9" t="inlineStr"/>
+      <c r="K100" s="9" t="inlineStr"/>
+      <c r="L100" s="9" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="M100" s="9" t="inlineStr">
+        <is>
+          <t>R3C8</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="B101" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C101" s="9" t="inlineStr">
+        <is>
+          <t>Door(L)</t>
+        </is>
+      </c>
+      <c r="D101" s="9" t="inlineStr">
+        <is>
+          <t>Cabinet Door</t>
+        </is>
+      </c>
+      <c r="E101" s="9" t="n">
+        <v>314.3</v>
+      </c>
+      <c r="F101" s="9" t="n">
+        <v>912.8</v>
+      </c>
+      <c r="G101" s="9" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="H101" s="9" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="I101" s="9" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="J101" s="9" t="inlineStr"/>
+      <c r="K101" s="9" t="inlineStr"/>
+      <c r="L101" s="9" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="M101" s="9" t="inlineStr">
+        <is>
+          <t>R3C10</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="B102" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C102" s="9" t="inlineStr">
+        <is>
+          <t>Door(L)</t>
+        </is>
+      </c>
+      <c r="D102" s="9" t="inlineStr">
+        <is>
+          <t>Cabinet Door</t>
+        </is>
+      </c>
+      <c r="E102" s="9" t="n">
+        <v>377.8</v>
+      </c>
+      <c r="F102" s="9" t="n">
+        <v>912.8</v>
+      </c>
+      <c r="G102" s="9" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="H102" s="9" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="I102" s="9" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="J102" s="9" t="inlineStr"/>
+      <c r="K102" s="9" t="inlineStr"/>
+      <c r="L102" s="9" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="M102" s="9" t="inlineStr">
+        <is>
+          <t>R3C7</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="B103" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C103" s="9" t="inlineStr">
+        <is>
+          <t>Door(L)</t>
+        </is>
+      </c>
+      <c r="D103" s="9" t="inlineStr">
+        <is>
+          <t>Cabinet Door</t>
+        </is>
+      </c>
+      <c r="E103" s="9" t="n">
+        <v>403.2</v>
+      </c>
+      <c r="F103" s="9" t="n">
+        <v>912.8</v>
+      </c>
+      <c r="G103" s="9" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="H103" s="9" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="I103" s="9" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="J103" s="9" t="inlineStr"/>
+      <c r="K103" s="9" t="inlineStr"/>
+      <c r="L103" s="9" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="M103" s="9" t="inlineStr">
+        <is>
+          <t>R3C9</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="B104" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C104" s="9" t="inlineStr">
+        <is>
+          <t>Door(L)</t>
+        </is>
+      </c>
+      <c r="D104" s="9" t="inlineStr">
+        <is>
+          <t>Cabinet Door</t>
+        </is>
+      </c>
+      <c r="E104" s="9" t="n">
+        <v>530.2</v>
+      </c>
+      <c r="F104" s="9" t="n">
+        <v>912.8</v>
+      </c>
+      <c r="G104" s="9" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="H104" s="9" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="I104" s="9" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="J104" s="9" t="inlineStr"/>
+      <c r="K104" s="9" t="inlineStr"/>
+      <c r="L104" s="9" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="M104" s="9" t="inlineStr">
+        <is>
+          <t>R3C11</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="B105" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C105" s="9" t="inlineStr">
+        <is>
+          <t>Door(L)</t>
+        </is>
+      </c>
+      <c r="D105" s="9" t="inlineStr">
+        <is>
+          <t>Cabinet Door</t>
+        </is>
+      </c>
+      <c r="E105" s="9" t="n">
+        <v>377.8</v>
+      </c>
+      <c r="F105" s="9" t="n">
+        <v>1446.2</v>
+      </c>
+      <c r="G105" s="9" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="H105" s="9" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="I105" s="9" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="J105" s="9" t="n">
+        <v>723.1</v>
+      </c>
+      <c r="K105" s="9" t="inlineStr"/>
+      <c r="L105" s="9" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="M105" s="9" t="inlineStr">
+        <is>
+          <t>R3C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="B106" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C106" s="9" t="inlineStr">
+        <is>
+          <t>Door(R)</t>
+        </is>
+      </c>
+      <c r="D106" s="9" t="inlineStr">
+        <is>
+          <t>Cabinet Door</t>
+        </is>
+      </c>
+      <c r="E106" s="9" t="n">
+        <v>435</v>
+      </c>
+      <c r="F106" s="9" t="n">
+        <v>606.4</v>
+      </c>
+      <c r="G106" s="9" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="H106" s="9" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
+      <c r="I106" s="9" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="J106" s="9" t="inlineStr"/>
+      <c r="K106" s="9" t="inlineStr"/>
+      <c r="L106" s="9" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="M106" s="9" t="inlineStr">
+        <is>
+          <t>R3C8</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="B107" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C107" s="9" t="inlineStr">
+        <is>
+          <t>Door(R)</t>
+        </is>
+      </c>
+      <c r="D107" s="9" t="inlineStr">
+        <is>
+          <t>Cabinet Door</t>
+        </is>
+      </c>
+      <c r="E107" s="9" t="n">
+        <v>403.2</v>
+      </c>
+      <c r="F107" s="9" t="n">
+        <v>912.8</v>
+      </c>
+      <c r="G107" s="9" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="H107" s="9" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
+      <c r="I107" s="9" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="J107" s="9" t="inlineStr"/>
+      <c r="K107" s="9" t="inlineStr"/>
+      <c r="L107" s="9" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="M107" s="9" t="inlineStr">
+        <is>
+          <t>R3C9</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="B108" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C108" s="9" t="inlineStr">
+        <is>
+          <t>Door(R)</t>
+        </is>
+      </c>
+      <c r="D108" s="9" t="inlineStr">
+        <is>
+          <t>Cabinet Door</t>
+        </is>
+      </c>
+      <c r="E108" s="9" t="n">
+        <v>631.8</v>
+      </c>
+      <c r="F108" s="9" t="n">
+        <v>912.8</v>
+      </c>
+      <c r="G108" s="9" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="H108" s="9" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
+      <c r="I108" s="9" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="J108" s="9" t="inlineStr"/>
+      <c r="K108" s="9" t="inlineStr"/>
+      <c r="L108" s="9" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="M108" s="9" t="inlineStr">
+        <is>
+          <t>R3C13</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="B109" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C109" s="7" t="inlineStr">
+        <is>
+          <t>Door(R)</t>
+        </is>
+      </c>
+      <c r="D109" s="7" t="inlineStr">
+        <is>
+          <t>Cabinet Door</t>
+        </is>
+      </c>
+      <c r="E109" s="7" t="n">
+        <v>377.8</v>
+      </c>
+      <c r="F109" s="7" t="n">
+        <v>1446.2</v>
+      </c>
+      <c r="G109" s="7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="H109" s="7" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
+      <c r="I109" s="7" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="J109" s="7" t="n">
+        <v>723.1</v>
+      </c>
+      <c r="K109" s="7" t="inlineStr"/>
+      <c r="L109" s="7" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="M109" s="7" t="inlineStr">
+        <is>
+          <t>R3C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="B110" s="8" t="inlineStr">
+        <is>
+          <t>Hinge Type Total: (12)</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="B113" s="10" t="inlineStr">
+        <is>
+          <t>Door Style Total: (13)</t>
+        </is>
+      </c>
+      <c r="C113" s="5" t="n"/>
+      <c r="D113" s="5" t="n"/>
+    </row>
+    <row r="115">
+      <c r="A115" s="11" t="inlineStr">
+        <is>
+          <t>Material Total: (13)</t>
+        </is>
+      </c>
+    </row>
+    <row r="116" ht="18" customHeight="1">
+      <c r="A116" s="2" t="inlineStr">
+        <is>
+          <t>02 - PAN - Absolute Acajou</t>
+        </is>
+      </c>
+    </row>
+    <row r="118" ht="18" customHeight="1">
+      <c r="A118" s="3" t="inlineStr">
+        <is>
+          <t>Shaker Door</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="B120" s="4" t="inlineStr">
+        <is>
+          <t>DTC C-80 110 / 2mm - 105-C80A675NF</t>
+        </is>
+      </c>
+      <c r="C120" s="5" t="n"/>
+      <c r="D120" s="5" t="n"/>
+      <c r="E120" s="5" t="n"/>
+      <c r="F120" s="5" t="n"/>
+      <c r="G120" s="5" t="n"/>
+      <c r="H120" s="5" t="n"/>
+      <c r="I120" s="5" t="n"/>
+      <c r="J120" s="5" t="n"/>
+      <c r="K120" s="5" t="n"/>
+      <c r="L120" s="5" t="n"/>
+      <c r="M120" s="5" t="n"/>
+    </row>
+    <row r="121">
+      <c r="B121" s="6" t="inlineStr">
+        <is>
+          <t>Qty</t>
+        </is>
+      </c>
+      <c r="C121" s="6" t="inlineStr">
+        <is>
+          <t>Door Name</t>
+        </is>
+      </c>
+      <c r="D121" s="6" t="inlineStr">
+        <is>
+          <t>Comment</t>
+        </is>
+      </c>
+      <c r="E121" s="6" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="F121" s="6" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="G121" s="6" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="H121" s="6" t="inlineStr">
+        <is>
+          <t>Edge</t>
+        </is>
+      </c>
+      <c r="I121" s="6" t="inlineStr">
+        <is>
+          <t>B/L</t>
+        </is>
+      </c>
+      <c r="J121" s="6" t="inlineStr">
+        <is>
+          <t>B2/L2</t>
+        </is>
+      </c>
+      <c r="K121" s="6" t="inlineStr">
+        <is>
+          <t>B3/L3</t>
+        </is>
+      </c>
+      <c r="L121" s="6" t="inlineStr">
+        <is>
+          <t>T/R</t>
+        </is>
+      </c>
+      <c r="M121" s="6" t="inlineStr">
+        <is>
+          <t>Cab #</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="B122" s="8" t="inlineStr">
+        <is>
+          <t>Hinge Type Total: (0)</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="B125" s="10" t="inlineStr">
+        <is>
+          <t>Door Style Total: (0)</t>
+        </is>
+      </c>
+      <c r="C125" s="5" t="n"/>
+      <c r="D125" s="5" t="n"/>
+    </row>
+    <row r="127" ht="18" customHeight="1">
+      <c r="A127" s="3" t="inlineStr">
         <is>
           <t>Slab Door - VG</t>
         </is>
       </c>
     </row>
-    <row r="100">
-      <c r="B100" s="4" t="inlineStr">
+    <row r="129">
+      <c r="B129" s="4" t="inlineStr">
         <is>
           <t>Blum 170 / 3mm - 71T658180</t>
         </is>
       </c>
-      <c r="C100" s="5" t="n"/>
-      <c r="D100" s="5" t="n"/>
-      <c r="E100" s="5" t="n"/>
-      <c r="F100" s="5" t="n"/>
-      <c r="G100" s="5" t="n"/>
-      <c r="H100" s="5" t="n"/>
-      <c r="I100" s="5" t="n"/>
-      <c r="J100" s="5" t="n"/>
-      <c r="K100" s="5" t="n"/>
-      <c r="L100" s="5" t="n"/>
-      <c r="M100" s="5" t="n"/>
-    </row>
-    <row r="101">
-      <c r="B101" s="6" t="inlineStr">
+      <c r="C129" s="5" t="n"/>
+      <c r="D129" s="5" t="n"/>
+      <c r="E129" s="5" t="n"/>
+      <c r="F129" s="5" t="n"/>
+      <c r="G129" s="5" t="n"/>
+      <c r="H129" s="5" t="n"/>
+      <c r="I129" s="5" t="n"/>
+      <c r="J129" s="5" t="n"/>
+      <c r="K129" s="5" t="n"/>
+      <c r="L129" s="5" t="n"/>
+      <c r="M129" s="5" t="n"/>
+    </row>
+    <row r="130">
+      <c r="B130" s="6" t="inlineStr">
         <is>
           <t>Qty</t>
         </is>
       </c>
-      <c r="C101" s="6" t="inlineStr">
+      <c r="C130" s="6" t="inlineStr">
         <is>
           <t>Door Name</t>
         </is>
       </c>
-      <c r="D101" s="6" t="inlineStr">
+      <c r="D130" s="6" t="inlineStr">
         <is>
           <t>Comment</t>
         </is>
       </c>
-      <c r="E101" s="6" t="inlineStr">
+      <c r="E130" s="6" t="inlineStr">
         <is>
           <t>W</t>
         </is>
       </c>
-      <c r="F101" s="6" t="inlineStr">
+      <c r="F130" s="6" t="inlineStr">
         <is>
           <t>H</t>
         </is>
       </c>
-      <c r="G101" s="6" t="inlineStr">
+      <c r="G130" s="6" t="inlineStr">
         <is>
           <t>Std</t>
         </is>
       </c>
-      <c r="H101" s="6" t="inlineStr">
+      <c r="H130" s="6" t="inlineStr">
         <is>
           <t>Edge</t>
         </is>
       </c>
-      <c r="I101" s="6" t="inlineStr">
+      <c r="I130" s="6" t="inlineStr">
         <is>
           <t>B/L</t>
         </is>
       </c>
-      <c r="J101" s="6" t="inlineStr">
+      <c r="J130" s="6" t="inlineStr">
         <is>
           <t>B2/L2</t>
         </is>
       </c>
-      <c r="K101" s="6" t="inlineStr">
-        <is>
-          <t>T2/R2</t>
-        </is>
-      </c>
-      <c r="L101" s="6" t="inlineStr">
+      <c r="K130" s="6" t="inlineStr">
+        <is>
+          <t>B3/L3</t>
+        </is>
+      </c>
+      <c r="L130" s="6" t="inlineStr">
         <is>
           <t>T/R</t>
         </is>
       </c>
-      <c r="M101" s="6" t="inlineStr">
+      <c r="M130" s="6" t="inlineStr">
         <is>
           <t>Cab #</t>
         </is>
       </c>
     </row>
-    <row r="102">
-      <c r="B102" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C102" s="7" t="inlineStr">
+    <row r="131">
+      <c r="B131" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C131" s="7" t="inlineStr">
         <is>
           <t>Door(L)</t>
         </is>
       </c>
-      <c r="D102" s="7" t="inlineStr">
-        <is>
-          <t>Cabinet Door</t>
-        </is>
-      </c>
-      <c r="E102" s="7" t="n">
+      <c r="D131" s="7" t="inlineStr">
+        <is>
+          <t>Cabinet Door</t>
+        </is>
+      </c>
+      <c r="E131" s="7" t="n">
         <v>279.4</v>
       </c>
-      <c r="F102" s="7" t="n">
+      <c r="F131" s="7" t="n">
         <v>771.5</v>
       </c>
-      <c r="G102" s="7" t="inlineStr">
+      <c r="G131" s="7" t="inlineStr">
         <is>
           <t>S</t>
         </is>
       </c>
-      <c r="H102" s="7" t="inlineStr">
+      <c r="H131" s="7" t="inlineStr">
         <is>
           <t>Left</t>
         </is>
       </c>
-      <c r="I102" s="7" t="n">
-        <v>101.6</v>
-      </c>
-      <c r="J102" s="7" t="inlineStr"/>
-      <c r="K102" s="7" t="inlineStr"/>
-      <c r="L102" s="7" t="n">
-        <v>101.6</v>
-      </c>
-      <c r="M102" s="7" t="inlineStr">
+      <c r="I131" s="7" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="J131" s="7" t="inlineStr"/>
+      <c r="K131" s="7" t="inlineStr"/>
+      <c r="L131" s="7" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="M131" s="7" t="inlineStr">
         <is>
           <t>R3C6</t>
         </is>
       </c>
     </row>
-    <row r="103">
-      <c r="B103" s="8" t="inlineStr">
+    <row r="132">
+      <c r="B132" s="8" t="inlineStr">
         <is>
           <t>Hinge Type Total: (1)</t>
         </is>
       </c>
     </row>
-    <row r="105">
-      <c r="B105" s="4" t="inlineStr">
+    <row r="134">
+      <c r="B134" s="4" t="inlineStr">
         <is>
           <t>Blum 95 Blind / 3mm - 79B958180</t>
         </is>
       </c>
-      <c r="C105" s="5" t="n"/>
-      <c r="D105" s="5" t="n"/>
-      <c r="E105" s="5" t="n"/>
-      <c r="F105" s="5" t="n"/>
-      <c r="G105" s="5" t="n"/>
-      <c r="H105" s="5" t="n"/>
-      <c r="I105" s="5" t="n"/>
-      <c r="J105" s="5" t="n"/>
-      <c r="K105" s="5" t="n"/>
-      <c r="L105" s="5" t="n"/>
-      <c r="M105" s="5" t="n"/>
-    </row>
-    <row r="106">
-      <c r="B106" s="6" t="inlineStr">
+      <c r="C134" s="5" t="n"/>
+      <c r="D134" s="5" t="n"/>
+      <c r="E134" s="5" t="n"/>
+      <c r="F134" s="5" t="n"/>
+      <c r="G134" s="5" t="n"/>
+      <c r="H134" s="5" t="n"/>
+      <c r="I134" s="5" t="n"/>
+      <c r="J134" s="5" t="n"/>
+      <c r="K134" s="5" t="n"/>
+      <c r="L134" s="5" t="n"/>
+      <c r="M134" s="5" t="n"/>
+    </row>
+    <row r="135">
+      <c r="B135" s="6" t="inlineStr">
         <is>
           <t>Qty</t>
         </is>
       </c>
-      <c r="C106" s="6" t="inlineStr">
+      <c r="C135" s="6" t="inlineStr">
         <is>
           <t>Door Name</t>
         </is>
       </c>
-      <c r="D106" s="6" t="inlineStr">
+      <c r="D135" s="6" t="inlineStr">
         <is>
           <t>Comment</t>
         </is>
       </c>
-      <c r="E106" s="6" t="inlineStr">
+      <c r="E135" s="6" t="inlineStr">
         <is>
           <t>W</t>
         </is>
       </c>
-      <c r="F106" s="6" t="inlineStr">
+      <c r="F135" s="6" t="inlineStr">
         <is>
           <t>H</t>
         </is>
       </c>
-      <c r="G106" s="6" t="inlineStr">
+      <c r="G135" s="6" t="inlineStr">
         <is>
           <t>Std</t>
         </is>
       </c>
-      <c r="H106" s="6" t="inlineStr">
+      <c r="H135" s="6" t="inlineStr">
         <is>
           <t>Edge</t>
         </is>
       </c>
-      <c r="I106" s="6" t="inlineStr">
+      <c r="I135" s="6" t="inlineStr">
         <is>
           <t>B/L</t>
         </is>
       </c>
-      <c r="J106" s="6" t="inlineStr">
+      <c r="J135" s="6" t="inlineStr">
         <is>
           <t>B2/L2</t>
         </is>
       </c>
-      <c r="K106" s="6" t="inlineStr">
-        <is>
-          <t>T2/R2</t>
-        </is>
-      </c>
-      <c r="L106" s="6" t="inlineStr">
+      <c r="K135" s="6" t="inlineStr">
+        <is>
+          <t>B3/L3</t>
+        </is>
+      </c>
+      <c r="L135" s="6" t="inlineStr">
         <is>
           <t>T/R</t>
         </is>
       </c>
-      <c r="M106" s="6" t="inlineStr">
+      <c r="M135" s="6" t="inlineStr">
         <is>
           <t>Cab #</t>
         </is>
       </c>
     </row>
-    <row r="107">
-      <c r="B107" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C107" s="7" t="inlineStr">
+    <row r="136">
+      <c r="B136" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C136" s="7" t="inlineStr">
         <is>
           <t>Door(L)</t>
         </is>
       </c>
-      <c r="D107" s="7" t="inlineStr">
-        <is>
-          <t>Cabinet Door</t>
-        </is>
-      </c>
-      <c r="E107" s="7" t="n">
+      <c r="D136" s="7" t="inlineStr">
+        <is>
+          <t>Cabinet Door</t>
+        </is>
+      </c>
+      <c r="E136" s="7" t="n">
         <v>479.4</v>
       </c>
-      <c r="F107" s="7" t="n">
+      <c r="F136" s="7" t="n">
         <v>771.5</v>
       </c>
-      <c r="G107" s="7" t="inlineStr">
+      <c r="G136" s="7" t="inlineStr">
         <is>
           <t>S</t>
         </is>
       </c>
-      <c r="H107" s="7" t="inlineStr">
+      <c r="H136" s="7" t="inlineStr">
         <is>
           <t>Left</t>
         </is>
       </c>
-      <c r="I107" s="7" t="n">
-        <v>101.6</v>
-      </c>
-      <c r="J107" s="7" t="inlineStr"/>
-      <c r="K107" s="7" t="inlineStr"/>
-      <c r="L107" s="7" t="n">
-        <v>101.6</v>
-      </c>
-      <c r="M107" s="7" t="inlineStr">
+      <c r="I136" s="7" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="J136" s="7" t="inlineStr"/>
+      <c r="K136" s="7" t="inlineStr"/>
+      <c r="L136" s="7" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="M136" s="7" t="inlineStr">
         <is>
           <t>R3C14</t>
         </is>
       </c>
     </row>
-    <row r="108">
-      <c r="B108" s="8" t="inlineStr">
+    <row r="137">
+      <c r="B137" s="8" t="inlineStr">
         <is>
           <t>Hinge Type Total: (1)</t>
         </is>
       </c>
     </row>
-    <row r="110">
-      <c r="B110" s="4" t="inlineStr">
+    <row r="139">
+      <c r="B139" s="4" t="inlineStr">
         <is>
           <t>Blum Bi-fold 60 / 0mm - 79T853180</t>
         </is>
       </c>
-      <c r="C110" s="5" t="n"/>
-      <c r="D110" s="5" t="n"/>
-      <c r="E110" s="5" t="n"/>
-      <c r="F110" s="5" t="n"/>
-      <c r="G110" s="5" t="n"/>
-      <c r="H110" s="5" t="n"/>
-      <c r="I110" s="5" t="n"/>
-      <c r="J110" s="5" t="n"/>
-      <c r="K110" s="5" t="n"/>
-      <c r="L110" s="5" t="n"/>
-      <c r="M110" s="5" t="n"/>
-    </row>
-    <row r="111">
-      <c r="B111" s="6" t="inlineStr">
+      <c r="C139" s="5" t="n"/>
+      <c r="D139" s="5" t="n"/>
+      <c r="E139" s="5" t="n"/>
+      <c r="F139" s="5" t="n"/>
+      <c r="G139" s="5" t="n"/>
+      <c r="H139" s="5" t="n"/>
+      <c r="I139" s="5" t="n"/>
+      <c r="J139" s="5" t="n"/>
+      <c r="K139" s="5" t="n"/>
+      <c r="L139" s="5" t="n"/>
+      <c r="M139" s="5" t="n"/>
+    </row>
+    <row r="140">
+      <c r="B140" s="6" t="inlineStr">
         <is>
           <t>Qty</t>
         </is>
       </c>
-      <c r="C111" s="6" t="inlineStr">
+      <c r="C140" s="6" t="inlineStr">
         <is>
           <t>Door Name</t>
         </is>
       </c>
-      <c r="D111" s="6" t="inlineStr">
+      <c r="D140" s="6" t="inlineStr">
         <is>
           <t>Comment</t>
         </is>
       </c>
-      <c r="E111" s="6" t="inlineStr">
+      <c r="E140" s="6" t="inlineStr">
         <is>
           <t>W</t>
         </is>
       </c>
-      <c r="F111" s="6" t="inlineStr">
+      <c r="F140" s="6" t="inlineStr">
         <is>
           <t>H</t>
         </is>
       </c>
-      <c r="G111" s="6" t="inlineStr">
+      <c r="G140" s="6" t="inlineStr">
         <is>
           <t>Std</t>
         </is>
       </c>
-      <c r="H111" s="6" t="inlineStr">
+      <c r="H140" s="6" t="inlineStr">
         <is>
           <t>Edge</t>
         </is>
       </c>
-      <c r="I111" s="6" t="inlineStr">
+      <c r="I140" s="6" t="inlineStr">
         <is>
           <t>B/L</t>
         </is>
       </c>
-      <c r="J111" s="6" t="inlineStr">
+      <c r="J140" s="6" t="inlineStr">
         <is>
           <t>B2/L2</t>
         </is>
       </c>
-      <c r="K111" s="6" t="inlineStr">
-        <is>
-          <t>T2/R2</t>
-        </is>
-      </c>
-      <c r="L111" s="6" t="inlineStr">
+      <c r="K140" s="6" t="inlineStr">
+        <is>
+          <t>B3/L3</t>
+        </is>
+      </c>
+      <c r="L140" s="6" t="inlineStr">
         <is>
           <t>T/R</t>
         </is>
       </c>
-      <c r="M111" s="6" t="inlineStr">
+      <c r="M140" s="6" t="inlineStr">
         <is>
           <t>Cab #</t>
         </is>
       </c>
     </row>
-    <row r="112">
-      <c r="B112" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C112" s="7" t="inlineStr">
+    <row r="141">
+      <c r="B141" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C141" s="7" t="inlineStr">
         <is>
           <t>Door(L)</t>
         </is>
       </c>
-      <c r="D112" s="7" t="inlineStr">
-        <is>
-          <t>Cabinet Door</t>
-        </is>
-      </c>
-      <c r="E112" s="7" t="n">
+      <c r="D141" s="7" t="inlineStr">
+        <is>
+          <t>Cabinet Door</t>
+        </is>
+      </c>
+      <c r="E141" s="7" t="n">
         <v>279.4</v>
       </c>
-      <c r="F112" s="7" t="n">
+      <c r="F141" s="7" t="n">
         <v>771.5</v>
       </c>
-      <c r="G112" s="7" t="inlineStr">
+      <c r="G141" s="7" t="inlineStr">
         <is>
           <t>S</t>
         </is>
       </c>
-      <c r="H112" s="7" t="inlineStr">
+      <c r="H141" s="7" t="inlineStr">
         <is>
           <t>Left</t>
         </is>
       </c>
-      <c r="I112" s="7" t="n">
-        <v>101.6</v>
-      </c>
-      <c r="J112" s="7" t="inlineStr"/>
-      <c r="K112" s="7" t="inlineStr"/>
-      <c r="L112" s="7" t="n">
-        <v>101.6</v>
-      </c>
-      <c r="M112" s="7" t="inlineStr">
+      <c r="I141" s="7" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="J141" s="7" t="inlineStr"/>
+      <c r="K141" s="7" t="inlineStr"/>
+      <c r="L141" s="7" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="M141" s="7" t="inlineStr">
         <is>
           <t>R3C6</t>
         </is>
       </c>
     </row>
-    <row r="113">
-      <c r="B113" s="8" t="inlineStr">
+    <row r="142">
+      <c r="B142" s="8" t="inlineStr">
         <is>
           <t>Hinge Type Total: (1)</t>
         </is>
       </c>
     </row>
-    <row r="115">
-      <c r="B115" s="4" t="inlineStr">
+    <row r="144">
+      <c r="B144" s="4" t="inlineStr">
         <is>
           <t>DTC C-80 110 / 2mm - 105-C80A675NF</t>
         </is>
       </c>
-      <c r="C115" s="5" t="n"/>
-      <c r="D115" s="5" t="n"/>
-      <c r="E115" s="5" t="n"/>
-      <c r="F115" s="5" t="n"/>
-      <c r="G115" s="5" t="n"/>
-      <c r="H115" s="5" t="n"/>
-      <c r="I115" s="5" t="n"/>
-      <c r="J115" s="5" t="n"/>
-      <c r="K115" s="5" t="n"/>
-      <c r="L115" s="5" t="n"/>
-      <c r="M115" s="5" t="n"/>
-    </row>
-    <row r="116">
-      <c r="B116" s="6" t="inlineStr">
+      <c r="C144" s="5" t="n"/>
+      <c r="D144" s="5" t="n"/>
+      <c r="E144" s="5" t="n"/>
+      <c r="F144" s="5" t="n"/>
+      <c r="G144" s="5" t="n"/>
+      <c r="H144" s="5" t="n"/>
+      <c r="I144" s="5" t="n"/>
+      <c r="J144" s="5" t="n"/>
+      <c r="K144" s="5" t="n"/>
+      <c r="L144" s="5" t="n"/>
+      <c r="M144" s="5" t="n"/>
+    </row>
+    <row r="145">
+      <c r="B145" s="6" t="inlineStr">
         <is>
           <t>Qty</t>
         </is>
       </c>
-      <c r="C116" s="6" t="inlineStr">
+      <c r="C145" s="6" t="inlineStr">
         <is>
           <t>Door Name</t>
         </is>
       </c>
-      <c r="D116" s="6" t="inlineStr">
+      <c r="D145" s="6" t="inlineStr">
         <is>
           <t>Comment</t>
         </is>
       </c>
-      <c r="E116" s="6" t="inlineStr">
+      <c r="E145" s="6" t="inlineStr">
         <is>
           <t>W</t>
         </is>
       </c>
-      <c r="F116" s="6" t="inlineStr">
+      <c r="F145" s="6" t="inlineStr">
         <is>
           <t>H</t>
         </is>
       </c>
-      <c r="G116" s="6" t="inlineStr">
+      <c r="G145" s="6" t="inlineStr">
         <is>
           <t>Std</t>
         </is>
       </c>
-      <c r="H116" s="6" t="inlineStr">
+      <c r="H145" s="6" t="inlineStr">
         <is>
           <t>Edge</t>
         </is>
       </c>
-      <c r="I116" s="6" t="inlineStr">
+      <c r="I145" s="6" t="inlineStr">
         <is>
           <t>B/L</t>
         </is>
       </c>
-      <c r="J116" s="6" t="inlineStr">
+      <c r="J145" s="6" t="inlineStr">
         <is>
           <t>B2/L2</t>
         </is>
       </c>
-      <c r="K116" s="6" t="inlineStr">
-        <is>
-          <t>T2/R2</t>
-        </is>
-      </c>
-      <c r="L116" s="6" t="inlineStr">
+      <c r="K145" s="6" t="inlineStr">
+        <is>
+          <t>B3/L3</t>
+        </is>
+      </c>
+      <c r="L145" s="6" t="inlineStr">
         <is>
           <t>T/R</t>
         </is>
       </c>
-      <c r="M116" s="6" t="inlineStr">
+      <c r="M145" s="6" t="inlineStr">
         <is>
           <t>Cab #</t>
         </is>
       </c>
     </row>
-    <row r="117">
-      <c r="B117" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C117" s="9" t="inlineStr">
+    <row r="146">
+      <c r="B146" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C146" s="9" t="inlineStr">
         <is>
           <t>Door(L)</t>
         </is>
       </c>
-      <c r="D117" s="9" t="inlineStr">
-        <is>
-          <t>Cabinet Door</t>
-        </is>
-      </c>
-      <c r="E117" s="9" t="n">
+      <c r="D146" s="9" t="inlineStr">
+        <is>
+          <t>Cabinet Door</t>
+        </is>
+      </c>
+      <c r="E146" s="9" t="n">
         <v>454</v>
       </c>
-      <c r="F117" s="9" t="n">
+      <c r="F146" s="9" t="n">
         <v>771.5</v>
       </c>
-      <c r="G117" s="9" t="inlineStr">
+      <c r="G146" s="9" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="H117" s="9" t="inlineStr">
+      <c r="H146" s="9" t="inlineStr">
         <is>
           <t>Left</t>
         </is>
       </c>
-      <c r="I117" s="9" t="n">
-        <v>101.6</v>
-      </c>
-      <c r="J117" s="9" t="inlineStr"/>
-      <c r="K117" s="9" t="inlineStr"/>
-      <c r="L117" s="9" t="n">
+      <c r="I146" s="9" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="J146" s="9" t="inlineStr"/>
+      <c r="K146" s="9" t="inlineStr"/>
+      <c r="L146" s="9" t="n">
         <v>228.6</v>
       </c>
-      <c r="M117" s="9" t="inlineStr">
+      <c r="M146" s="9" t="inlineStr">
         <is>
           <t>R3C4</t>
         </is>
       </c>
     </row>
-    <row r="118">
-      <c r="B118" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C118" s="7" t="inlineStr">
+    <row r="147">
+      <c r="B147" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C147" s="7" t="inlineStr">
         <is>
           <t>Door(R)</t>
         </is>
       </c>
-      <c r="D118" s="7" t="inlineStr">
-        <is>
-          <t>Cabinet Door</t>
-        </is>
-      </c>
-      <c r="E118" s="7" t="n">
+      <c r="D147" s="7" t="inlineStr">
+        <is>
+          <t>Cabinet Door</t>
+        </is>
+      </c>
+      <c r="E147" s="7" t="n">
         <v>454</v>
       </c>
-      <c r="F118" s="7" t="n">
+      <c r="F147" s="7" t="n">
         <v>771.5</v>
       </c>
-      <c r="G118" s="7" t="inlineStr">
+      <c r="G147" s="7" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="H118" s="7" t="inlineStr">
+      <c r="H147" s="7" t="inlineStr">
         <is>
           <t>Right</t>
         </is>
       </c>
-      <c r="I118" s="7" t="n">
-        <v>101.6</v>
-      </c>
-      <c r="J118" s="7" t="inlineStr"/>
-      <c r="K118" s="7" t="inlineStr"/>
-      <c r="L118" s="7" t="n">
+      <c r="I147" s="7" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="J147" s="7" t="inlineStr"/>
+      <c r="K147" s="7" t="inlineStr"/>
+      <c r="L147" s="7" t="n">
         <v>228.6</v>
       </c>
-      <c r="M118" s="7" t="inlineStr">
+      <c r="M147" s="7" t="inlineStr">
         <is>
           <t>R3C4</t>
         </is>
       </c>
     </row>
-    <row r="119">
-      <c r="B119" s="8" t="inlineStr">
+    <row r="148">
+      <c r="B148" s="8" t="inlineStr">
         <is>
           <t>Hinge Type Total: (2)</t>
         </is>
       </c>
     </row>
-    <row r="122">
-      <c r="B122" s="10" t="inlineStr">
+    <row r="151">
+      <c r="B151" s="10" t="inlineStr">
         <is>
           <t>Door Style Total: (5)</t>
         </is>
       </c>
-      <c r="C122" s="5" t="n"/>
-      <c r="D122" s="5" t="n"/>
-    </row>
-    <row r="124">
-      <c r="A124" s="11" t="inlineStr">
+      <c r="C151" s="5" t="n"/>
+      <c r="D151" s="5" t="n"/>
+    </row>
+    <row r="153">
+      <c r="A153" s="11" t="inlineStr">
         <is>
           <t>Material Total: (5)</t>
         </is>
       </c>
     </row>
-    <row r="125" ht="18" customHeight="1">
-      <c r="A125" s="2" t="inlineStr">
+    <row r="154" ht="18" customHeight="1">
+      <c r="A154" s="2" t="inlineStr">
         <is>
           <t>3-4 TBD</t>
         </is>
       </c>
     </row>
-    <row r="127">
-      <c r="A127" s="11" t="inlineStr">
+    <row r="156">
+      <c r="A156" s="11" t="inlineStr">
         <is>
           <t>Material Total: (0)</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="43">
+  <mergeCells count="51">
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A2:M2"/>
     <mergeCell ref="A4:M4"/>
@@ -3665,21 +4445,29 @@
     <mergeCell ref="A87:M87"/>
     <mergeCell ref="A89:M89"/>
     <mergeCell ref="B91:M91"/>
-    <mergeCell ref="B93:M93"/>
+    <mergeCell ref="B94:M94"/>
     <mergeCell ref="B96:M96"/>
-    <mergeCell ref="A98:M98"/>
-    <mergeCell ref="B100:M100"/>
-    <mergeCell ref="B103:M103"/>
-    <mergeCell ref="B105:M105"/>
-    <mergeCell ref="B108:M108"/>
     <mergeCell ref="B110:M110"/>
     <mergeCell ref="B113:M113"/>
-    <mergeCell ref="B115:M115"/>
-    <mergeCell ref="B119:M119"/>
+    <mergeCell ref="A115:L115"/>
+    <mergeCell ref="A116:M116"/>
+    <mergeCell ref="A118:M118"/>
+    <mergeCell ref="B120:M120"/>
     <mergeCell ref="B122:M122"/>
-    <mergeCell ref="A124:L124"/>
-    <mergeCell ref="A125:M125"/>
-    <mergeCell ref="A127:L127"/>
+    <mergeCell ref="B125:M125"/>
+    <mergeCell ref="A127:M127"/>
+    <mergeCell ref="B129:M129"/>
+    <mergeCell ref="B132:M132"/>
+    <mergeCell ref="B134:M134"/>
+    <mergeCell ref="B137:M137"/>
+    <mergeCell ref="B139:M139"/>
+    <mergeCell ref="B142:M142"/>
+    <mergeCell ref="B144:M144"/>
+    <mergeCell ref="B148:M148"/>
+    <mergeCell ref="B151:M151"/>
+    <mergeCell ref="A153:L153"/>
+    <mergeCell ref="A154:M154"/>
+    <mergeCell ref="A156:L156"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.25"/>
   <pageSetup fitToHeight="0"/>
@@ -3691,11 +4479,12 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
-  <rowBreaks count="4" manualBreakCount="4">
+  <rowBreaks count="5" manualBreakCount="5">
     <brk id="44" min="0" max="16383" man="1"/>
     <brk id="86" min="0" max="16383" man="1"/>
-    <brk id="124" min="0" max="16383" man="1"/>
-    <brk id="127" min="0" max="16383" man="1"/>
+    <brk id="115" min="0" max="16383" man="1"/>
+    <brk id="153" min="0" max="16383" man="1"/>
+    <brk id="156" min="0" max="16383" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>